<commit_message>
updated, random coordinate location still wrong
</commit_message>
<xml_diff>
--- a/results/REopt_data.xlsx
+++ b/results/REopt_data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results0" r:id="rId4" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -16,6 +17,83 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+  <si>
+    <t>input_Latitude</t>
+  </si>
+  <si>
+    <t>input_Longitude</t>
+  </si>
+  <si>
+    <t>input_PV_location</t>
+  </si>
+  <si>
+    <t>input_PV_installed_cost</t>
+  </si>
+  <si>
+    <t>input_Wind_installed_cost</t>
+  </si>
+  <si>
+    <t>input_Site_electric_load</t>
+  </si>
+  <si>
+    <t>input_Site_building_type</t>
+  </si>
+  <si>
+    <t>input_Site_roofspace</t>
+  </si>
+  <si>
+    <t>input_Site_landspace</t>
+  </si>
+  <si>
+    <t>input_Site_NEM_limit</t>
+  </si>
+  <si>
+    <t>input_Site_net_billing_rate</t>
+  </si>
+  <si>
+    <t>input_Site_electricity_cost_per_kwh</t>
+  </si>
+  <si>
+    <t>input_Site_demand_charge_cost_per_kw</t>
+  </si>
+  <si>
+    <t>output_PV_size</t>
+  </si>
+  <si>
+    <t>output_PV_energy_lcoe</t>
+  </si>
+  <si>
+    <t>output_PV_energy_exported</t>
+  </si>
+  <si>
+    <t>output_PV_energy_curtailed</t>
+  </si>
+  <si>
+    <t>output_Wind_size</t>
+  </si>
+  <si>
+    <t>output_Wind_energy_lcoe</t>
+  </si>
+  <si>
+    <t>output_Wind_energy_exported</t>
+  </si>
+  <si>
+    <t>output_Wind_energy_curtailed</t>
+  </si>
+  <si>
+    <t>output_Grid_Electricity_Supplied_kWh_annual</t>
+  </si>
+  <si>
+    <t>output_npv</t>
+  </si>
+  <si>
+    <t>output_lcc</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -339,4 +417,165 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.0</v>
+      </c>
+      <c r="E2">
+        <v>0.0</v>
+      </c>
+      <c r="F2">
+        <v>0.0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.0</v>
+      </c>
+      <c r="I2">
+        <v>0.0</v>
+      </c>
+      <c r="J2">
+        <v>0.0</v>
+      </c>
+      <c r="K2">
+        <v>0.0</v>
+      </c>
+      <c r="L2">
+        <v>0.0</v>
+      </c>
+      <c r="M2">
+        <v>0.0</v>
+      </c>
+      <c r="N2">
+        <v>455.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>275124.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>61.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>24737.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>20155.0</v>
+      </c>
+      <c r="W2">
+        <v>2.04436131e6</v>
+      </c>
+      <c r="X2">
+        <v>1.52072871e6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated script, run this one
</commit_message>
<xml_diff>
--- a/results/REopt_data.xlsx
+++ b/results/REopt_data.xlsx
@@ -8,15 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbernal\Documents\GitHub\Public_REopt_analysis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83CF833-8331-4417-A306-416DD4DC4493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473BB230-DE5F-4BBD-889A-CF4E5614B460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Results0" sheetId="2" r:id="rId2"/>
     <sheet name="Results1" sheetId="3" r:id="rId3"/>
     <sheet name="Results2" sheetId="4" r:id="rId4"/>
+    <sheet name="Results3" sheetId="5" r:id="rId5"/>
+    <sheet name="Results4" r:id="rId9" sheetId="6"/>
+    <sheet name="Results5" r:id="rId10" sheetId="7"/>
+    <sheet name="Results6" r:id="rId11" sheetId="8"/>
+    <sheet name="v2_Results0" r:id="rId12" sheetId="9"/>
+    <sheet name="v2_Results1" r:id="rId13" sheetId="10"/>
+    <sheet name="v2_Results2" r:id="rId14" sheetId="11"/>
+    <sheet name="v2_Results3" r:id="rId15" sheetId="12"/>
+    <sheet name="v2_Results4" r:id="rId16" sheetId="13"/>
+    <sheet name="v2_Results5" r:id="rId17" sheetId="14"/>
+    <sheet name="v2_Results6" r:id="rId18" sheetId="15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>input_Latitude</t>
   </si>
@@ -106,6 +117,39 @@
   </si>
   <si>
     <t>StripMall</t>
+  </si>
+  <si>
+    <t>roof</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>SmallOffice</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>FlatLoad_16_5</t>
+  </si>
+  <si>
+    <t>Supermarket</t>
+  </si>
+  <si>
+    <t>PrimarySchool</t>
+  </si>
+  <si>
+    <t>SecondarySchool</t>
+  </si>
+  <si>
+    <t>FullServiceRest</t>
+  </si>
+  <si>
+    <t>FlatLoad_8_5</t>
   </si>
 </sst>
 </file>
@@ -426,12 +470,1422 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E940BFE6-CC7E-405F-A6DD-9A78C9B47AD9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>45.37951553</v>
+      </c>
+      <c r="B2">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>3704.91</v>
+      </c>
+      <c r="E2">
+        <v>5602.94</v>
+      </c>
+      <c r="F2">
+        <v>1.812605e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2">
+        <v>778927.0</v>
+      </c>
+      <c r="I2">
+        <v>5.0</v>
+      </c>
+      <c r="J2">
+        <v>400.0</v>
+      </c>
+      <c r="K2">
+        <v>0.09</v>
+      </c>
+      <c r="L2">
+        <v>0.14</v>
+      </c>
+      <c r="M2">
+        <v>174.42</v>
+      </c>
+      <c r="N2">
+        <v>1877.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>2.010293e6</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>39.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>16746.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>1.773409e6</v>
+      </c>
+      <c r="W2">
+        <v>1.73240499e6</v>
+      </c>
+      <c r="X2">
+        <v>5.8891322e6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>3704.91</v>
+      </c>
+      <c r="E3">
+        <v>5602.94</v>
+      </c>
+      <c r="F3">
+        <v>1.812605e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3">
+        <v>778927.0</v>
+      </c>
+      <c r="I3">
+        <v>5.0</v>
+      </c>
+      <c r="J3">
+        <v>400.0</v>
+      </c>
+      <c r="K3">
+        <v>0.09</v>
+      </c>
+      <c r="L3">
+        <v>0.14</v>
+      </c>
+      <c r="M3">
+        <v>174.42</v>
+      </c>
+      <c r="N3">
+        <v>701.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>337079.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>564.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>898161.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>427821.0</v>
+      </c>
+      <c r="W3">
+        <v>2.34478763e6</v>
+      </c>
+      <c r="X3">
+        <v>1.090803319e7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.0</v>
+      </c>
+      <c r="E2">
+        <v>0.0</v>
+      </c>
+      <c r="F2">
+        <v>0.0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.0</v>
+      </c>
+      <c r="I2">
+        <v>0.0</v>
+      </c>
+      <c r="J2">
+        <v>0.0</v>
+      </c>
+      <c r="K2">
+        <v>0.0</v>
+      </c>
+      <c r="L2">
+        <v>0.0</v>
+      </c>
+      <c r="M2">
+        <v>0.0</v>
+      </c>
+      <c r="N2">
+        <v>50.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>24293.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>0.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>1.765886e6</v>
+      </c>
+      <c r="W2">
+        <v>2493.42</v>
+      </c>
+      <c r="X2">
+        <v>6.47580122e6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.0</v>
+      </c>
+      <c r="E3">
+        <v>0.0</v>
+      </c>
+      <c r="F3">
+        <v>0.0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.0</v>
+      </c>
+      <c r="I3">
+        <v>0.0</v>
+      </c>
+      <c r="J3">
+        <v>0.0</v>
+      </c>
+      <c r="K3">
+        <v>0.0</v>
+      </c>
+      <c r="L3">
+        <v>0.0</v>
+      </c>
+      <c r="M3">
+        <v>0.0</v>
+      </c>
+      <c r="N3">
+        <v>118.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>14161.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>906.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>1.347474e6</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>1.361635e6</v>
+      </c>
+      <c r="W3">
+        <v>3.53986077e6</v>
+      </c>
+      <c r="X3">
+        <v>1.767459233e7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>45.37951553</v>
+      </c>
+      <c r="B2">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>2526.02</v>
+      </c>
+      <c r="E2">
+        <v>5267.45</v>
+      </c>
+      <c r="F2">
+        <v>2.002177e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2">
+        <v>123277.0</v>
+      </c>
+      <c r="I2">
+        <v>7.0</v>
+      </c>
+      <c r="J2">
+        <v>400.0</v>
+      </c>
+      <c r="K2">
+        <v>0.04</v>
+      </c>
+      <c r="L2">
+        <v>0.05</v>
+      </c>
+      <c r="M2">
+        <v>249.08</v>
+      </c>
+      <c r="N2">
+        <v>1230.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>559196.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>0.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>2.822328e6</v>
+      </c>
+      <c r="W2">
+        <v>1.59496447e6</v>
+      </c>
+      <c r="X2">
+        <v>1.049188789e7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>2526.02</v>
+      </c>
+      <c r="E3">
+        <v>5267.45</v>
+      </c>
+      <c r="F3">
+        <v>2.002177e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>123277.0</v>
+      </c>
+      <c r="I3">
+        <v>7.0</v>
+      </c>
+      <c r="J3">
+        <v>400.0</v>
+      </c>
+      <c r="K3">
+        <v>0.04</v>
+      </c>
+      <c r="L3">
+        <v>0.05</v>
+      </c>
+      <c r="M3">
+        <v>249.08</v>
+      </c>
+      <c r="N3">
+        <v>1233.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>762819.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>434.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>601609.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>487954.0</v>
+      </c>
+      <c r="W3">
+        <v>3.017312e6</v>
+      </c>
+      <c r="X3">
+        <v>1.72316873e7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>45.37951553</v>
+      </c>
+      <c r="B2">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>3906.27</v>
+      </c>
+      <c r="E2">
+        <v>5030.53</v>
+      </c>
+      <c r="F2">
+        <v>4.235446e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2">
+        <v>871750.0</v>
+      </c>
+      <c r="I2">
+        <v>0.0</v>
+      </c>
+      <c r="J2">
+        <v>50.0</v>
+      </c>
+      <c r="K2">
+        <v>0.01</v>
+      </c>
+      <c r="L2">
+        <v>0.06</v>
+      </c>
+      <c r="M2">
+        <v>183.79</v>
+      </c>
+      <c r="N2">
+        <v>0.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>0.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>0.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>3.280674e6</v>
+      </c>
+      <c r="W2">
+        <v>0.0</v>
+      </c>
+      <c r="X2">
+        <v>7.81943515e6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>3906.27</v>
+      </c>
+      <c r="E3">
+        <v>5030.53</v>
+      </c>
+      <c r="F3">
+        <v>4.235446e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3">
+        <v>871750.0</v>
+      </c>
+      <c r="I3">
+        <v>0.0</v>
+      </c>
+      <c r="J3">
+        <v>50.0</v>
+      </c>
+      <c r="K3">
+        <v>0.01</v>
+      </c>
+      <c r="L3">
+        <v>0.06</v>
+      </c>
+      <c r="M3">
+        <v>183.79</v>
+      </c>
+      <c r="N3">
+        <v>201.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>0.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>215.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>1025.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>3.318828e6</v>
+      </c>
+      <c r="W3">
+        <v>522278.48</v>
+      </c>
+      <c r="X3">
+        <v>1.99048114e7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>45.37951553</v>
+      </c>
+      <c r="B2">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>4019.38</v>
+      </c>
+      <c r="E2">
+        <v>2985.3</v>
+      </c>
+      <c r="F2">
+        <v>4.997114e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>270663.0</v>
+      </c>
+      <c r="I2">
+        <v>3.0</v>
+      </c>
+      <c r="J2">
+        <v>3500.0</v>
+      </c>
+      <c r="K2">
+        <v>0.05</v>
+      </c>
+      <c r="L2">
+        <v>0.11</v>
+      </c>
+      <c r="M2">
+        <v>116.9</v>
+      </c>
+      <c r="N2">
+        <v>52.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>10752.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>395.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>525566.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>536318.0</v>
+      </c>
+      <c r="W2">
+        <v>182652.25</v>
+      </c>
+      <c r="X2">
+        <v>2.90867484e6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>4019.38</v>
+      </c>
+      <c r="E3">
+        <v>2985.3</v>
+      </c>
+      <c r="F3">
+        <v>4.997114e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>270663.0</v>
+      </c>
+      <c r="I3">
+        <v>3.0</v>
+      </c>
+      <c r="J3">
+        <v>3500.0</v>
+      </c>
+      <c r="K3">
+        <v>0.05</v>
+      </c>
+      <c r="L3">
+        <v>0.11</v>
+      </c>
+      <c r="M3">
+        <v>116.9</v>
+      </c>
+      <c r="N3">
+        <v>507.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>58573.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>1410.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>2.016006e6</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>2.074579e6</v>
+      </c>
+      <c r="W3">
+        <v>4.0305516e6</v>
+      </c>
+      <c r="X3">
+        <v>2.029681383e7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>37.66811942</v>
+      </c>
+      <c r="B2">
+        <v>-105.5247554</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>2706.49</v>
+      </c>
+      <c r="E2">
+        <v>6521.87</v>
+      </c>
+      <c r="F2">
+        <v>408979.0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2">
+        <v>942664.0</v>
+      </c>
+      <c r="I2">
+        <v>3.0</v>
+      </c>
+      <c r="J2">
+        <v>3500.0</v>
+      </c>
+      <c r="K2">
+        <v>0.02</v>
+      </c>
+      <c r="L2">
+        <v>0.11</v>
+      </c>
+      <c r="M2">
+        <v>16.14</v>
+      </c>
+      <c r="N2">
+        <v>245.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>162554.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>0.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>162554.0</v>
+      </c>
+      <c r="W2">
+        <v>100353.0</v>
+      </c>
+      <c r="X2">
+        <v>807218.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>3682.72</v>
+      </c>
+      <c r="E3">
+        <v>4085.16</v>
+      </c>
+      <c r="F3">
+        <v>1.406697e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>942664.0</v>
+      </c>
+      <c r="I3">
+        <v>10.0</v>
+      </c>
+      <c r="J3">
+        <v>750.0</v>
+      </c>
+      <c r="K3">
+        <v>0.03</v>
+      </c>
+      <c r="L3">
+        <v>0.14</v>
+      </c>
+      <c r="M3">
+        <v>84.38</v>
+      </c>
+      <c r="N3">
+        <v>129.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>26424.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>402.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>553689.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>580113.0</v>
+      </c>
+      <c r="W3">
+        <v>1.23917783e6</v>
+      </c>
+      <c r="X3">
+        <v>4.65099562e6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -442,9 +1896,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +1972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -603,9 +2057,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +2133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -753,7 +2207,7 @@
         <v>1364855.65</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -827,7 +2281,7 @@
         <v>10125997.09</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -910,87 +2364,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2295EDE-7FDA-4DAB-8989-134A1ED5CE6D}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:24" ht="75" dyDescent="0.25" s="1" customFormat="1">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s" s="1">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s" s="1">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s" s="1">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s" s="1">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s" s="1">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s" s="1">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s" s="1">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s" s="1">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s" s="1">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s" s="1">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s" s="1">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s" s="1">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s" s="1">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s" s="1">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s" s="1">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s" s="1">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" t="s" s="1">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" t="s" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" dyDescent="0.25">
       <c r="A2">
         <v>37.668119419999996</v>
       </c>
@@ -1062,6 +2516,1331 @@
       </c>
       <c r="X2">
         <v>1669677.72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" ht="75" dyDescent="0.25" s="1" customFormat="1">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s" s="1">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s" s="1">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s" s="1">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s" s="1">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s" s="1">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s" s="1">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" dyDescent="0.25">
+      <c r="A2">
+        <v>36.544681439999998</v>
+      </c>
+      <c r="B2">
+        <v>-86.244898849999998</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>2354.0100000000002</v>
+      </c>
+      <c r="E2">
+        <v>6093.24</v>
+      </c>
+      <c r="F2">
+        <v>4589077</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>357994</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>300</v>
+      </c>
+      <c r="K2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L2">
+        <v>0.09</v>
+      </c>
+      <c r="M2">
+        <v>199.73</v>
+      </c>
+      <c r="N2">
+        <v>493</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>45790</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>79</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>10166</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>427451</v>
+      </c>
+      <c r="W2">
+        <v>935962.18</v>
+      </c>
+      <c r="X2">
+        <v>3188080.67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" dyDescent="0.25">
+      <c r="A3">
+        <v>36.544681439999998</v>
+      </c>
+      <c r="B3">
+        <v>-86.244898849999998</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>2354.0100000000002</v>
+      </c>
+      <c r="E3">
+        <v>6093.24</v>
+      </c>
+      <c r="F3">
+        <v>4589077</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3">
+        <v>357994</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>300</v>
+      </c>
+      <c r="K3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.09</v>
+      </c>
+      <c r="M3">
+        <v>199.73</v>
+      </c>
+      <c r="N3">
+        <v>858</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>160485</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>884</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>742925</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>564502</v>
+      </c>
+      <c r="W3">
+        <v>18573246.640000001</v>
+      </c>
+      <c r="X3">
+        <v>13636762.060000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" dyDescent="0.25">
+      <c r="A4">
+        <v>36.544681439999998</v>
+      </c>
+      <c r="B4">
+        <v>-86.244898849999998</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>2354.0100000000002</v>
+      </c>
+      <c r="E4">
+        <v>6093.24</v>
+      </c>
+      <c r="F4">
+        <v>4589077</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>357994</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>300</v>
+      </c>
+      <c r="K4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.09</v>
+      </c>
+      <c r="M4">
+        <v>199.73</v>
+      </c>
+      <c r="N4">
+        <v>3580</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>2008991</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>1161</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1118337</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>72684</v>
+      </c>
+      <c r="W4">
+        <v>11817209.460000001</v>
+      </c>
+      <c r="X4">
+        <v>12915501.289999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X4"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>36.54468144</v>
+      </c>
+      <c r="B2">
+        <v>-86.24489885</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>3858.28</v>
+      </c>
+      <c r="E2">
+        <v>6461.39</v>
+      </c>
+      <c r="F2">
+        <v>4.156441e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>206562.0</v>
+      </c>
+      <c r="I2">
+        <v>5.0</v>
+      </c>
+      <c r="J2">
+        <v>300.0</v>
+      </c>
+      <c r="K2">
+        <v>0.03</v>
+      </c>
+      <c r="L2">
+        <v>0.04</v>
+      </c>
+      <c r="M2">
+        <v>121.16</v>
+      </c>
+      <c r="N2">
+        <v>1299.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>427261.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>866.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>700469.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>1.12773e6</v>
+      </c>
+      <c r="W2">
+        <v>8.43410382e6</v>
+      </c>
+      <c r="X2">
+        <v>1.10953431e7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>36.54468144</v>
+      </c>
+      <c r="B3">
+        <v>-86.24489885</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>3858.28</v>
+      </c>
+      <c r="E3">
+        <v>6461.39</v>
+      </c>
+      <c r="F3">
+        <v>4.156441e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3">
+        <v>206562.0</v>
+      </c>
+      <c r="I3">
+        <v>5.0</v>
+      </c>
+      <c r="J3">
+        <v>300.0</v>
+      </c>
+      <c r="K3">
+        <v>0.03</v>
+      </c>
+      <c r="L3">
+        <v>0.04</v>
+      </c>
+      <c r="M3">
+        <v>121.16</v>
+      </c>
+      <c r="N3">
+        <v>489.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>270061.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>262.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>204367.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>25229.0</v>
+      </c>
+      <c r="W3">
+        <v>959167.21</v>
+      </c>
+      <c r="X3">
+        <v>3.05316596e6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4">
+        <v>36.54468144</v>
+      </c>
+      <c r="B4">
+        <v>-86.24489885</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>3858.28</v>
+      </c>
+      <c r="E4">
+        <v>6461.39</v>
+      </c>
+      <c r="F4">
+        <v>4.156441e6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4">
+        <v>206562.0</v>
+      </c>
+      <c r="I4">
+        <v>5.0</v>
+      </c>
+      <c r="J4">
+        <v>300.0</v>
+      </c>
+      <c r="K4">
+        <v>0.03</v>
+      </c>
+      <c r="L4">
+        <v>0.04</v>
+      </c>
+      <c r="M4">
+        <v>121.16</v>
+      </c>
+      <c r="N4">
+        <v>1088.0</v>
+      </c>
+      <c r="O4">
+        <v>0.0</v>
+      </c>
+      <c r="P4">
+        <v>22432.0</v>
+      </c>
+      <c r="Q4">
+        <v>0.0</v>
+      </c>
+      <c r="R4">
+        <v>266.0</v>
+      </c>
+      <c r="S4">
+        <v>0.0</v>
+      </c>
+      <c r="T4">
+        <v>7634.0</v>
+      </c>
+      <c r="U4">
+        <v>0.0</v>
+      </c>
+      <c r="V4">
+        <v>2.106831e6</v>
+      </c>
+      <c r="W4">
+        <v>6.0190387e6</v>
+      </c>
+      <c r="X4">
+        <v>1.359682819e7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>45.37951553</v>
+      </c>
+      <c r="B2">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>3770.62</v>
+      </c>
+      <c r="E2">
+        <v>6430.31</v>
+      </c>
+      <c r="F2">
+        <v>1.324321e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <v>0.0</v>
+      </c>
+      <c r="I2">
+        <v>6.0</v>
+      </c>
+      <c r="J2">
+        <v>100.0</v>
+      </c>
+      <c r="K2">
+        <v>0.12</v>
+      </c>
+      <c r="L2">
+        <v>0.14</v>
+      </c>
+      <c r="M2">
+        <v>41.54</v>
+      </c>
+      <c r="N2">
+        <v>59.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>0.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>-0.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>4.385496e6</v>
+      </c>
+      <c r="W2">
+        <v>72837.18</v>
+      </c>
+      <c r="X2">
+        <v>7.95592026e6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>3770.62</v>
+      </c>
+      <c r="E3">
+        <v>6430.31</v>
+      </c>
+      <c r="F3">
+        <v>1.324321e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3">
+        <v>0.0</v>
+      </c>
+      <c r="I3">
+        <v>6.0</v>
+      </c>
+      <c r="J3">
+        <v>100.0</v>
+      </c>
+      <c r="K3">
+        <v>0.12</v>
+      </c>
+      <c r="L3">
+        <v>0.14</v>
+      </c>
+      <c r="M3">
+        <v>41.54</v>
+      </c>
+      <c r="N3">
+        <v>30.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>1090.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>70.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>4641.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>1.081917e6</v>
+      </c>
+      <c r="W3">
+        <v>235689.18</v>
+      </c>
+      <c r="X3">
+        <v>3.55835918e6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>45.37951553</v>
+      </c>
+      <c r="B2">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>3678.6</v>
+      </c>
+      <c r="E2">
+        <v>3243.95</v>
+      </c>
+      <c r="F2">
+        <v>2.318899e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2">
+        <v>357212.0</v>
+      </c>
+      <c r="I2">
+        <v>8.0</v>
+      </c>
+      <c r="J2">
+        <v>0.0</v>
+      </c>
+      <c r="K2">
+        <v>0.06</v>
+      </c>
+      <c r="L2">
+        <v>0.06</v>
+      </c>
+      <c r="M2">
+        <v>194.18</v>
+      </c>
+      <c r="N2">
+        <v>1141.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>1.181199e6</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>-0.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>1.181199e6</v>
+      </c>
+      <c r="W2">
+        <v>406773.68</v>
+      </c>
+      <c r="X2">
+        <v>1.042383205e7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>3678.6</v>
+      </c>
+      <c r="E3">
+        <v>3243.95</v>
+      </c>
+      <c r="F3">
+        <v>2.318899e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3">
+        <v>357212.0</v>
+      </c>
+      <c r="I3">
+        <v>8.0</v>
+      </c>
+      <c r="J3">
+        <v>0.0</v>
+      </c>
+      <c r="K3">
+        <v>0.06</v>
+      </c>
+      <c r="L3">
+        <v>0.06</v>
+      </c>
+      <c r="M3">
+        <v>194.18</v>
+      </c>
+      <c r="N3">
+        <v>0.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>0.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>0.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>0.0</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>2.318899e6</v>
+      </c>
+      <c r="W3">
+        <v>0.0</v>
+      </c>
+      <c r="X3">
+        <v>1.567758341e7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2">
+        <v>45.37951553</v>
+      </c>
+      <c r="B2">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>3096.62</v>
+      </c>
+      <c r="E2">
+        <v>5683.07</v>
+      </c>
+      <c r="F2">
+        <v>3.376688e6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>847212.0</v>
+      </c>
+      <c r="I2">
+        <v>1.0</v>
+      </c>
+      <c r="J2">
+        <v>2000.0</v>
+      </c>
+      <c r="K2">
+        <v>0.02</v>
+      </c>
+      <c r="L2">
+        <v>0.13</v>
+      </c>
+      <c r="M2">
+        <v>229.61</v>
+      </c>
+      <c r="N2">
+        <v>0.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>0.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>-0.0</v>
+      </c>
+      <c r="S2">
+        <v>0.0</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+      <c r="U2">
+        <v>0.0</v>
+      </c>
+      <c r="V2">
+        <v>673762.0</v>
+      </c>
+      <c r="W2">
+        <v>0.0</v>
+      </c>
+      <c r="X2">
+        <v>3.87214797e6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3">
+        <v>45.37951553</v>
+      </c>
+      <c r="B3">
+        <v>-91.4646535</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>3096.62</v>
+      </c>
+      <c r="E3">
+        <v>5683.07</v>
+      </c>
+      <c r="F3">
+        <v>3.376688e6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>847212.0</v>
+      </c>
+      <c r="I3">
+        <v>1.0</v>
+      </c>
+      <c r="J3">
+        <v>2000.0</v>
+      </c>
+      <c r="K3">
+        <v>0.02</v>
+      </c>
+      <c r="L3">
+        <v>0.13</v>
+      </c>
+      <c r="M3">
+        <v>229.61</v>
+      </c>
+      <c r="N3">
+        <v>113.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3">
+        <v>14438.0</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>1045.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>1.406578e6</v>
+      </c>
+      <c r="U3">
+        <v>0.0</v>
+      </c>
+      <c r="V3">
+        <v>1.421016e6</v>
+      </c>
+      <c r="W3">
+        <v>2.67219841e6</v>
+      </c>
+      <c r="X3">
+        <v>2.1046366e7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected how to see all REopt inputs
</commit_message>
<xml_diff>
--- a/results/REopt_data.xlsx
+++ b/results/REopt_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbernal\Documents\GitHub\Public_REopt_analysis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473BB230-DE5F-4BBD-889A-CF4E5614B460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B448C7-CD6E-4F80-A3AE-952BDD93C49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,17 @@
     <sheet name="Results1" sheetId="3" r:id="rId3"/>
     <sheet name="Results2" sheetId="4" r:id="rId4"/>
     <sheet name="Results3" sheetId="5" r:id="rId5"/>
-    <sheet name="Results4" r:id="rId9" sheetId="6"/>
-    <sheet name="Results5" r:id="rId10" sheetId="7"/>
-    <sheet name="Results6" r:id="rId11" sheetId="8"/>
-    <sheet name="v2_Results0" r:id="rId12" sheetId="9"/>
-    <sheet name="v2_Results1" r:id="rId13" sheetId="10"/>
-    <sheet name="v2_Results2" r:id="rId14" sheetId="11"/>
-    <sheet name="v2_Results3" r:id="rId15" sheetId="12"/>
-    <sheet name="v2_Results4" r:id="rId16" sheetId="13"/>
-    <sheet name="v2_Results5" r:id="rId17" sheetId="14"/>
-    <sheet name="v2_Results6" r:id="rId18" sheetId="15"/>
+    <sheet name="Results4" sheetId="6" r:id="rId6"/>
+    <sheet name="Results5" sheetId="7" r:id="rId7"/>
+    <sheet name="Results6" sheetId="8" r:id="rId8"/>
+    <sheet name="v2_Results0" sheetId="9" r:id="rId9"/>
+    <sheet name="v2_Results1" sheetId="10" r:id="rId10"/>
+    <sheet name="v2_Results2" sheetId="11" r:id="rId11"/>
+    <sheet name="v2_Results3" sheetId="12" r:id="rId12"/>
+    <sheet name="v2_Results4" sheetId="13" r:id="rId13"/>
+    <sheet name="v2_Results5" sheetId="14" r:id="rId14"/>
+    <sheet name="v2_Results6" sheetId="15" r:id="rId15"/>
+    <sheet name="v2_Results7" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="39">
   <si>
     <t>input_Latitude</t>
   </si>
@@ -150,6 +151,12 @@
   </si>
   <si>
     <t>FlatLoad_8_5</t>
+  </si>
+  <si>
+    <t>SmallHotel</t>
+  </si>
+  <si>
+    <t>MediumOffice</t>
   </si>
 </sst>
 </file>
@@ -469,8 +476,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E940BFE6-CC7E-405F-A6DD-9A78C9B47AD9}">
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D48FE19-2B90-411B-A12E-BD42D909BA94}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -481,14 +488,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B748D5-E5E6-4C9A-AD5F-00893A684CF8}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,12 +569,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B2">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -579,69 +586,69 @@
         <v>5602.94</v>
       </c>
       <c r="F2">
-        <v>1.812605e6</v>
+        <v>1812605</v>
       </c>
       <c r="G2" t="s">
         <v>33</v>
       </c>
       <c r="H2">
-        <v>778927.0</v>
+        <v>778927</v>
       </c>
       <c r="I2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="K2">
         <v>0.09</v>
       </c>
       <c r="L2">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M2">
         <v>174.42</v>
       </c>
       <c r="N2">
-        <v>1877.0</v>
+        <v>1877</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>2.010293e6</v>
+        <v>2010293</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>16746.0</v>
+        <v>16746</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1.773409e6</v>
+        <v>1773409</v>
       </c>
       <c r="W2">
-        <v>1.73240499e6</v>
+        <v>1732404.99</v>
       </c>
       <c r="X2">
-        <v>5.8891322e6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>5889132.2000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -653,61 +660,61 @@
         <v>5602.94</v>
       </c>
       <c r="F3">
-        <v>1.812605e6</v>
+        <v>1812605</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
       </c>
       <c r="H3">
-        <v>778927.0</v>
+        <v>778927</v>
       </c>
       <c r="I3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="K3">
         <v>0.09</v>
       </c>
       <c r="L3">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M3">
         <v>174.42</v>
       </c>
       <c r="N3">
-        <v>701.0</v>
+        <v>701</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>337079.0</v>
+        <v>337079</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>564.0</v>
+        <v>564</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>898161.0</v>
+        <v>898161</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>427821.0</v>
+        <v>427821</v>
       </c>
       <c r="W3">
-        <v>2.34478763e6</v>
+        <v>2344787.63</v>
       </c>
       <c r="X3">
-        <v>1.090803319e7</v>
+        <v>10908033.189999999</v>
       </c>
     </row>
   </sheetData>
@@ -716,14 +723,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D35AC5-DE34-42EF-BA07-BDD46ACCC4E8}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -797,7 +804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -808,70 +815,70 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>24293.0</v>
+        <v>24293</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1.765886e6</v>
+        <v>1765886</v>
       </c>
       <c r="W2">
         <v>2493.42</v>
       </c>
       <c r="X2">
-        <v>6.47580122e6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>6475801.2199999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -882,67 +889,67 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>118.0</v>
+        <v>118</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>14161.0</v>
+        <v>14161</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>906.0</v>
+        <v>906</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>1.347474e6</v>
+        <v>1347474</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1.361635e6</v>
+        <v>1361635</v>
       </c>
       <c r="W3">
-        <v>3.53986077e6</v>
+        <v>3539860.77</v>
       </c>
       <c r="X3">
-        <v>1.767459233e7</v>
+        <v>17674592.329999998</v>
       </c>
     </row>
   </sheetData>
@@ -951,14 +958,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30FB527B-0733-49E6-8D82-4695747A0EB8}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1032,12 +1039,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B2">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -1049,19 +1056,19 @@
         <v>5267.45</v>
       </c>
       <c r="F2">
-        <v>2.002177e6</v>
+        <v>2002177</v>
       </c>
       <c r="G2" t="s">
         <v>34</v>
       </c>
       <c r="H2">
-        <v>123277.0</v>
+        <v>123277</v>
       </c>
       <c r="I2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="J2">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="K2">
         <v>0.04</v>
@@ -1073,45 +1080,45 @@
         <v>249.08</v>
       </c>
       <c r="N2">
-        <v>1230.0</v>
+        <v>1230</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>559196.0</v>
+        <v>559196</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>2.822328e6</v>
+        <v>2822328</v>
       </c>
       <c r="W2">
-        <v>1.59496447e6</v>
+        <v>1594964.47</v>
       </c>
       <c r="X2">
-        <v>1.049188789e7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>10491887.890000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -1123,19 +1130,19 @@
         <v>5267.45</v>
       </c>
       <c r="F3">
-        <v>2.002177e6</v>
+        <v>2002177</v>
       </c>
       <c r="G3" t="s">
         <v>34</v>
       </c>
       <c r="H3">
-        <v>123277.0</v>
+        <v>123277</v>
       </c>
       <c r="I3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="K3">
         <v>0.04</v>
@@ -1147,37 +1154,37 @@
         <v>249.08</v>
       </c>
       <c r="N3">
-        <v>1233.0</v>
+        <v>1233</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>762819.0</v>
+        <v>762819</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>434.0</v>
+        <v>434</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>601609.0</v>
+        <v>601609</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>487954.0</v>
+        <v>487954</v>
       </c>
       <c r="W3">
-        <v>3.017312e6</v>
+        <v>3017312</v>
       </c>
       <c r="X3">
-        <v>1.72316873e7</v>
+        <v>17231687.300000001</v>
       </c>
     </row>
   </sheetData>
@@ -1186,14 +1193,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8659296B-C81F-4B03-B89E-0E79793DCC05}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1267,12 +1274,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B2">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1284,19 +1291,19 @@
         <v>5030.53</v>
       </c>
       <c r="F2">
-        <v>4.235446e6</v>
+        <v>4235446</v>
       </c>
       <c r="G2" t="s">
         <v>35</v>
       </c>
       <c r="H2">
-        <v>871750.0</v>
+        <v>871750</v>
       </c>
       <c r="I2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="K2">
         <v>0.01</v>
@@ -1308,45 +1315,45 @@
         <v>183.79</v>
       </c>
       <c r="N2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>3.280674e6</v>
+        <v>3280674</v>
       </c>
       <c r="W2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>7.81943515e6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>7819435.1500000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -1358,19 +1365,19 @@
         <v>5030.53</v>
       </c>
       <c r="F3">
-        <v>4.235446e6</v>
+        <v>4235446</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
       </c>
       <c r="H3">
-        <v>871750.0</v>
+        <v>871750</v>
       </c>
       <c r="I3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="K3">
         <v>0.01</v>
@@ -1382,37 +1389,37 @@
         <v>183.79</v>
       </c>
       <c r="N3">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>215.0</v>
+        <v>215</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>1025.0</v>
+        <v>1025</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>3.318828e6</v>
+        <v>3318828</v>
       </c>
       <c r="W3">
         <v>522278.48</v>
       </c>
       <c r="X3">
-        <v>1.99048114e7</v>
+        <v>19904811.399999999</v>
       </c>
     </row>
   </sheetData>
@@ -1421,14 +1428,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE6840F-4DFF-42F4-909B-AB83D8F7BF00}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1502,12 +1509,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B2">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1519,19 +1526,19 @@
         <v>2985.3</v>
       </c>
       <c r="F2">
-        <v>4.997114e6</v>
+        <v>4997114</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
       </c>
       <c r="H2">
-        <v>270663.0</v>
+        <v>270663</v>
       </c>
       <c r="I2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>3500.0</v>
+        <v>3500</v>
       </c>
       <c r="K2">
         <v>0.05</v>
@@ -1543,45 +1550,45 @@
         <v>116.9</v>
       </c>
       <c r="N2">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>10752.0</v>
+        <v>10752</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>395.0</v>
+        <v>395</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>525566.0</v>
+        <v>525566</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>536318.0</v>
+        <v>536318</v>
       </c>
       <c r="W2">
         <v>182652.25</v>
       </c>
       <c r="X2">
-        <v>2.90867484e6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>2908674.84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -1593,19 +1600,19 @@
         <v>2985.3</v>
       </c>
       <c r="F3">
-        <v>4.997114e6</v>
+        <v>4997114</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
       </c>
       <c r="H3">
-        <v>270663.0</v>
+        <v>270663</v>
       </c>
       <c r="I3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>3500.0</v>
+        <v>3500</v>
       </c>
       <c r="K3">
         <v>0.05</v>
@@ -1617,37 +1624,37 @@
         <v>116.9</v>
       </c>
       <c r="N3">
-        <v>507.0</v>
+        <v>507</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>58573.0</v>
+        <v>58573</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>1410.0</v>
+        <v>1410</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>2.016006e6</v>
+        <v>2016006</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>2.074579e6</v>
+        <v>2074579</v>
       </c>
       <c r="W3">
-        <v>4.0305516e6</v>
+        <v>4030551.6</v>
       </c>
       <c r="X3">
-        <v>2.029681383e7</v>
+        <v>20296813.829999998</v>
       </c>
     </row>
   </sheetData>
@@ -1656,14 +1663,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1DC106-40E3-4C69-B145-FF8822639ED8}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1737,9 +1744,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>37.66811942</v>
+        <v>37.668119419999996</v>
       </c>
       <c r="B2">
         <v>-105.5247554</v>
@@ -1754,19 +1761,19 @@
         <v>6521.87</v>
       </c>
       <c r="F2">
-        <v>408979.0</v>
+        <v>408979</v>
       </c>
       <c r="G2" t="s">
         <v>36</v>
       </c>
       <c r="H2">
-        <v>942664.0</v>
+        <v>942664</v>
       </c>
       <c r="I2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J2">
-        <v>3500.0</v>
+        <v>3500</v>
       </c>
       <c r="K2">
         <v>0.02</v>
@@ -1778,45 +1785,45 @@
         <v>16.14</v>
       </c>
       <c r="N2">
-        <v>245.0</v>
+        <v>245</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>162554.0</v>
+        <v>162554</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>162554.0</v>
+        <v>162554</v>
       </c>
       <c r="W2">
-        <v>100353.0</v>
+        <v>100353</v>
       </c>
       <c r="X2">
         <v>807218.81</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -1828,61 +1835,446 @@
         <v>4085.16</v>
       </c>
       <c r="F3">
-        <v>1.406697e6</v>
+        <v>1406697</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
       </c>
       <c r="H3">
-        <v>942664.0</v>
+        <v>942664</v>
       </c>
       <c r="I3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="J3">
-        <v>750.0</v>
+        <v>750</v>
       </c>
       <c r="K3">
         <v>0.03</v>
       </c>
       <c r="L3">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M3">
         <v>84.38</v>
       </c>
       <c r="N3">
-        <v>129.0</v>
+        <v>129</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>26424.0</v>
+        <v>26424</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>402.0</v>
+        <v>402</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>553689.0</v>
+        <v>553689</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>580113.0</v>
+        <v>580113</v>
       </c>
       <c r="W3">
-        <v>1.23917783e6</v>
+        <v>1239177.83</v>
       </c>
       <c r="X3">
-        <v>4.65099562e6</v>
+        <v>4650995.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B3A8D0-FBAC-4A3E-8701-ABE5574EE7BE}">
+  <dimension ref="A1:X5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>37.668119419999996</v>
+      </c>
+      <c r="B2">
+        <v>-105.5247554</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>2600.3000000000002</v>
+      </c>
+      <c r="E2">
+        <v>7752.11</v>
+      </c>
+      <c r="F2">
+        <v>950100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2">
+        <v>84258</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>0.11</v>
+      </c>
+      <c r="L2">
+        <v>0.15</v>
+      </c>
+      <c r="M2">
+        <v>113.64</v>
+      </c>
+      <c r="N2">
+        <v>843</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>888811</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>4921</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>407768</v>
+      </c>
+      <c r="W2">
+        <v>791061.76</v>
+      </c>
+      <c r="X2">
+        <v>3317925.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>45.379515529999999</v>
+      </c>
+      <c r="B3">
+        <v>-91.464653499999997</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>4171.99</v>
+      </c>
+      <c r="E3">
+        <v>5418.46</v>
+      </c>
+      <c r="F3">
+        <v>3144377</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3">
+        <v>84258</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>5000</v>
+      </c>
+      <c r="K3">
+        <v>0.08</v>
+      </c>
+      <c r="L3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M3">
+        <v>128.51</v>
+      </c>
+      <c r="N3">
+        <v>190</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>31757</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>939</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1156890</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>1188647</v>
+      </c>
+      <c r="W3">
+        <v>1989500.54</v>
+      </c>
+      <c r="X3">
+        <v>11834908.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>36.544681439999998</v>
+      </c>
+      <c r="B4">
+        <v>-86.244898849999998</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>3757.64</v>
+      </c>
+      <c r="E4">
+        <v>3317.37</v>
+      </c>
+      <c r="F4">
+        <v>2553602</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4">
+        <v>406582</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>4000</v>
+      </c>
+      <c r="K4">
+        <v>0.01</v>
+      </c>
+      <c r="L4">
+        <v>0.01</v>
+      </c>
+      <c r="M4">
+        <v>32.57</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>14</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>2516460</v>
+      </c>
+      <c r="W4">
+        <v>2400.48</v>
+      </c>
+      <c r="X4">
+        <v>2463547.31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>36.511206629999997</v>
+      </c>
+      <c r="B5">
+        <v>-110.61968090000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>3085.45</v>
+      </c>
+      <c r="E5">
+        <v>4852.9399999999996</v>
+      </c>
+      <c r="F5">
+        <v>4016818</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>154777</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>5000</v>
+      </c>
+      <c r="K5">
+        <v>0.03</v>
+      </c>
+      <c r="L5">
+        <v>0.04</v>
+      </c>
+      <c r="M5">
+        <v>209.84</v>
+      </c>
+      <c r="N5">
+        <v>389</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>47693</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>202</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>20387</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>2925833</v>
+      </c>
+      <c r="W5">
+        <v>1627972.19</v>
+      </c>
+      <c r="X5">
+        <v>34408400.840000004</v>
       </c>
     </row>
   </sheetData>
@@ -1891,14 +2283,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46435D0D-C54A-447F-9BAB-8EE2EC53C01E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62F069FC-78AD-470F-B61B-8690677520D6}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +2364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2052,14 +2444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DF2252-1FE0-477A-83C6-AF4972764882}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D798797C-F542-4A73-86D6-D8A68419E777}">
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2133,7 +2525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2207,7 +2599,7 @@
         <v>1364855.65</v>
       </c>
     </row>
-    <row r="3" spans="1:24" dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2281,7 +2673,7 @@
         <v>10125997.09</v>
       </c>
     </row>
-    <row r="4" spans="1:24" dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2361,7 +2753,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2295EDE-7FDA-4DAB-8989-134A1ED5CE6D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CC18E52-7803-4201-8E89-146A3651D711}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2370,81 +2762,81 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="75" dyDescent="0.25" s="1" customFormat="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>37.668119419999996</v>
       </c>
@@ -2524,90 +2916,90 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F8F484-10CC-4AC2-BA18-B52CF8105E3B}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" ht="75" dyDescent="0.25" s="1" customFormat="1">
-      <c r="A1" t="s" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="1">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="1">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="1">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="1">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="1">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="1">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="1">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="1">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="1">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="1">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="1">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s" s="1">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s" s="1">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="1">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s" s="1">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s" s="1">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>36.544681439999998</v>
       </c>
@@ -2681,7 +3073,7 @@
         <v>3188080.67</v>
       </c>
     </row>
-    <row r="3" spans="1:24" dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>36.544681439999998</v>
       </c>
@@ -2755,7 +3147,7 @@
         <v>13636762.060000001</v>
       </c>
     </row>
-    <row r="4" spans="1:24" dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>36.544681439999998</v>
       </c>
@@ -2835,14 +3227,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1341F8EF-68D7-464A-9498-52239B14A072}">
   <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2916,12 +3308,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>36.54468144</v>
+        <v>36.544681439999998</v>
       </c>
       <c r="B2">
-        <v>-86.24489885</v>
+        <v>-86.244898849999998</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -2933,19 +3325,19 @@
         <v>6461.39</v>
       </c>
       <c r="F2">
-        <v>4.156441e6</v>
+        <v>4156441</v>
       </c>
       <c r="G2" t="s">
         <v>28</v>
       </c>
       <c r="H2">
-        <v>206562.0</v>
+        <v>206562</v>
       </c>
       <c r="I2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="K2">
         <v>0.03</v>
@@ -2957,45 +3349,45 @@
         <v>121.16</v>
       </c>
       <c r="N2">
-        <v>1299.0</v>
+        <v>1299</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>427261.0</v>
+        <v>427261</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>866.0</v>
+        <v>866</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>700469.0</v>
+        <v>700469</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1.12773e6</v>
+        <v>1127730</v>
       </c>
       <c r="W2">
-        <v>8.43410382e6</v>
+        <v>8434103.8200000003</v>
       </c>
       <c r="X2">
-        <v>1.10953431e7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>11095343.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>36.54468144</v>
+        <v>36.544681439999998</v>
       </c>
       <c r="B3">
-        <v>-86.24489885</v>
+        <v>-86.244898849999998</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -3007,19 +3399,19 @@
         <v>6461.39</v>
       </c>
       <c r="F3">
-        <v>4.156441e6</v>
+        <v>4156441</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
       </c>
       <c r="H3">
-        <v>206562.0</v>
+        <v>206562</v>
       </c>
       <c r="I3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="K3">
         <v>0.03</v>
@@ -3031,45 +3423,45 @@
         <v>121.16</v>
       </c>
       <c r="N3">
-        <v>489.0</v>
+        <v>489</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>270061.0</v>
+        <v>270061</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>262.0</v>
+        <v>262</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>204367.0</v>
+        <v>204367</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>25229.0</v>
+        <v>25229</v>
       </c>
       <c r="W3">
         <v>959167.21</v>
       </c>
       <c r="X3">
-        <v>3.05316596e6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+        <v>3053165.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>36.54468144</v>
+        <v>36.544681439999998</v>
       </c>
       <c r="B4">
-        <v>-86.24489885</v>
+        <v>-86.244898849999998</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -3081,19 +3473,19 @@
         <v>6461.39</v>
       </c>
       <c r="F4">
-        <v>4.156441e6</v>
+        <v>4156441</v>
       </c>
       <c r="G4" t="s">
         <v>28</v>
       </c>
       <c r="H4">
-        <v>206562.0</v>
+        <v>206562</v>
       </c>
       <c r="I4">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J4">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="K4">
         <v>0.03</v>
@@ -3105,37 +3497,37 @@
         <v>121.16</v>
       </c>
       <c r="N4">
-        <v>1088.0</v>
+        <v>1088</v>
       </c>
       <c r="O4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>22432.0</v>
+        <v>22432</v>
       </c>
       <c r="Q4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>266.0</v>
+        <v>266</v>
       </c>
       <c r="S4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>7634.0</v>
+        <v>7634</v>
       </c>
       <c r="U4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>2.106831e6</v>
+        <v>2106831</v>
       </c>
       <c r="W4">
-        <v>6.0190387e6</v>
+        <v>6019038.7000000002</v>
       </c>
       <c r="X4">
-        <v>1.359682819e7</v>
+        <v>13596828.189999999</v>
       </c>
     </row>
   </sheetData>
@@ -3144,14 +3536,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5EC928-D36B-40EC-80C3-63BF430EF923}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3225,12 +3617,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B2">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -3242,69 +3634,69 @@
         <v>6430.31</v>
       </c>
       <c r="F2">
-        <v>1.324321e6</v>
+        <v>1324321</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
       </c>
       <c r="H2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="J2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>0.12</v>
       </c>
       <c r="L2">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M2">
         <v>41.54</v>
       </c>
       <c r="N2">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>4.385496e6</v>
+        <v>4385496</v>
       </c>
       <c r="W2">
-        <v>72837.18</v>
+        <v>72837.179999999993</v>
       </c>
       <c r="X2">
-        <v>7.95592026e6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>7955920.2599999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -3316,61 +3708,61 @@
         <v>6430.31</v>
       </c>
       <c r="F3">
-        <v>1.324321e6</v>
+        <v>1324321</v>
       </c>
       <c r="G3" t="s">
         <v>29</v>
       </c>
       <c r="H3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="J3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="K3">
         <v>0.12</v>
       </c>
       <c r="L3">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M3">
         <v>41.54</v>
       </c>
       <c r="N3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>1090.0</v>
+        <v>1090</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>4641.0</v>
+        <v>4641</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1.081917e6</v>
+        <v>1081917</v>
       </c>
       <c r="W3">
         <v>235689.18</v>
       </c>
       <c r="X3">
-        <v>3.55835918e6</v>
+        <v>3558359.18</v>
       </c>
     </row>
   </sheetData>
@@ -3379,14 +3771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1E7CFF-D2AE-4DF2-8E58-854C7B1C59DD}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3460,12 +3852,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B2">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -3477,19 +3869,19 @@
         <v>3243.95</v>
       </c>
       <c r="F2">
-        <v>2.318899e6</v>
+        <v>2318899</v>
       </c>
       <c r="G2" t="s">
         <v>31</v>
       </c>
       <c r="H2">
-        <v>357212.0</v>
+        <v>357212</v>
       </c>
       <c r="I2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="J2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0.06</v>
@@ -3501,45 +3893,45 @@
         <v>194.18</v>
       </c>
       <c r="N2">
-        <v>1141.0</v>
+        <v>1141</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>1.181199e6</v>
+        <v>1181199</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1.181199e6</v>
+        <v>1181199</v>
       </c>
       <c r="W2">
         <v>406773.68</v>
       </c>
       <c r="X2">
-        <v>1.042383205e7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>10423832.050000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -3551,19 +3943,19 @@
         <v>3243.95</v>
       </c>
       <c r="F3">
-        <v>2.318899e6</v>
+        <v>2318899</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
       </c>
       <c r="H3">
-        <v>357212.0</v>
+        <v>357212</v>
       </c>
       <c r="I3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="J3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0.06</v>
@@ -3575,37 +3967,37 @@
         <v>194.18</v>
       </c>
       <c r="N3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>2.318899e6</v>
+        <v>2318899</v>
       </c>
       <c r="W3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>1.567758341e7</v>
+        <v>15677583.41</v>
       </c>
     </row>
   </sheetData>
@@ -3614,14 +4006,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C72AA02-E690-4E73-B651-072483C4C064}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3695,12 +4087,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B2">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -3712,19 +4104,19 @@
         <v>5683.07</v>
       </c>
       <c r="F2">
-        <v>3.376688e6</v>
+        <v>3376688</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
       </c>
       <c r="H2">
-        <v>847212.0</v>
+        <v>847212</v>
       </c>
       <c r="I2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="K2">
         <v>0.02</v>
@@ -3736,45 +4128,45 @@
         <v>229.61</v>
       </c>
       <c r="N2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>-0.0</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>673762.0</v>
+        <v>673762</v>
       </c>
       <c r="W2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>3.87214797e6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+        <v>3872147.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45.37951553</v>
+        <v>45.379515529999999</v>
       </c>
       <c r="B3">
-        <v>-91.4646535</v>
+        <v>-91.464653499999997</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
@@ -3786,19 +4178,19 @@
         <v>5683.07</v>
       </c>
       <c r="F3">
-        <v>3.376688e6</v>
+        <v>3376688</v>
       </c>
       <c r="G3" t="s">
         <v>32</v>
       </c>
       <c r="H3">
-        <v>847212.0</v>
+        <v>847212</v>
       </c>
       <c r="I3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>2000.0</v>
+        <v>2000</v>
       </c>
       <c r="K3">
         <v>0.02</v>
@@ -3810,40 +4202,46 @@
         <v>229.61</v>
       </c>
       <c r="N3">
-        <v>113.0</v>
+        <v>113</v>
       </c>
       <c r="O3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="P3">
-        <v>14438.0</v>
+        <v>14438</v>
       </c>
       <c r="Q3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>1045.0</v>
+        <v>1045</v>
       </c>
       <c r="S3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>1.406578e6</v>
+        <v>1406578</v>
       </c>
       <c r="U3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>1.421016e6</v>
+        <v>1421016</v>
       </c>
       <c r="W3">
-        <v>2.67219841e6</v>
+        <v>2672198.41</v>
       </c>
       <c r="X3">
-        <v>2.1046366e7</v>
+        <v>21046366</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>